<commit_message>
Updated formulas. Near completion
</commit_message>
<xml_diff>
--- a/amazon.xlsx
+++ b/amazon.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kerrs\Desktop\Excel-Exercises\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kerrs\Desktop\Amazon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87708F99-38C8-46F6-A022-7D633A22209E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6F2C3E-18CD-4236-8A81-8D0E982FAAEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{09650164-32A5-5E41-B315-3AC4BDEF06DC}"/>
   </bookViews>
@@ -121,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -129,6 +129,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,7 +448,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="107" zoomScaleNormal="177" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -502,7 +504,9 @@
       <c r="H3" s="5">
         <v>232887</v>
       </c>
-      <c r="I3" s="4"/>
+      <c r="I3" s="7">
+        <v>0.31</v>
+      </c>
       <c r="J3">
         <f>(E3-B3)/B3 * 100</f>
         <v>30.796326119408473</v>
@@ -512,12 +516,12 @@
         <v>30.93396152159491</v>
       </c>
       <c r="L3">
-        <f>H3 *(1 + 0.2)</f>
-        <v>279464.39999999997</v>
+        <f>H3 *(1 + I3)</f>
+        <v>305081.97000000003</v>
       </c>
       <c r="M3">
-        <f>L3 *(1+ 0.2)</f>
-        <v>335357.27999999997</v>
+        <f>L3 *(1+ I3)</f>
+        <v>399657.38070000004</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -558,7 +562,9 @@
       <c r="H6" s="5">
         <v>139156</v>
       </c>
-      <c r="I6" s="4"/>
+      <c r="I6" s="7">
+        <v>0.22</v>
+      </c>
       <c r="J6">
         <f>(E6-B6) /B6 * 100</f>
         <v>26.815838667648556</v>
@@ -568,8 +574,12 @@
         <v>24.319688387799953</v>
       </c>
       <c r="L6">
-        <f>H6/(1 + 2.5)</f>
-        <v>39758.857142857145</v>
+        <f>H6*(1 + I6)</f>
+        <v>169770.32</v>
+      </c>
+      <c r="M6">
+        <f>L6*(1 + I6)</f>
+        <v>207119.7904</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -600,7 +610,9 @@
       <c r="H8" s="5">
         <v>13814</v>
       </c>
-      <c r="I8" s="4"/>
+      <c r="I8" s="7">
+        <v>0.35</v>
+      </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="4"/>
@@ -620,6 +632,14 @@
         <f>(H8-E8)/E8 * 100</f>
         <v>37.193365776144603</v>
       </c>
+      <c r="L9" s="8">
+        <f>H8*(1+I8)</f>
+        <v>18648.900000000001</v>
+      </c>
+      <c r="M9">
+        <f>L9*(1 + I8)</f>
+        <v>25176.015000000003</v>
+      </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="4" t="s">
@@ -903,54 +923,51 @@
     </row>
   </sheetData>
   <mergeCells count="111">
-    <mergeCell ref="I29:I30"/>
-    <mergeCell ref="J29:J30"/>
-    <mergeCell ref="K29:K30"/>
-    <mergeCell ref="L29:L30"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="I14:I15"/>
@@ -969,51 +986,54 @@
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="H16:H17"/>
     <mergeCell ref="I16:I17"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="K29:K30"/>
+    <mergeCell ref="L29:L30"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>